<commit_message>
planilha de resolucao problema kart
</commit_message>
<xml_diff>
--- a/Problema de Kart.xlsx
+++ b/Problema de Kart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Área de Trabalho\Problema Kart\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -552,6 +552,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,19 +601,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
@@ -984,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="K2" s="28">
-        <f t="shared" ref="K2:K7" si="1">E2+E10+E18+E26</f>
+        <f t="shared" ref="K2:K6" si="1">E2+E10+E18+E26</f>
         <v>2.9117824074074076E-3</v>
       </c>
       <c r="L2" s="30">
@@ -1256,11 +1256,11 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E8" s="19"/>
-      <c r="J8" s="45" t="s">
+      <c r="J8" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="34" t="s">
         <v>52</v>
       </c>
@@ -1534,12 +1534,12 @@
       <c r="H15" s="9">
         <v>0.99559791666666664</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J16" s="40">
@@ -1574,12 +1574,12 @@
       <c r="H17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
@@ -1636,12 +1636,12 @@
       <c r="H19" s="10">
         <v>0.9939650000000001</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="J19" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -1700,12 +1700,12 @@
       <c r="H21" s="10">
         <v>0.99400184027777783</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="44"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="44"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1730,14 +1730,14 @@
       <c r="H22" s="10">
         <v>0.99429040509259259</v>
       </c>
-      <c r="J22" s="58" t="s">
+      <c r="J22" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="K22" s="59">
+      <c r="K22" s="47">
         <f>G2+K2</f>
         <v>0.99464123842592589</v>
       </c>
-      <c r="L22" s="57"/>
+      <c r="L22" s="45"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1765,23 +1765,23 @@
       <c r="J23" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="56">
-        <f t="shared" ref="K23:K27" si="8">G3+K3</f>
+      <c r="K23" s="44">
+        <f t="shared" ref="K23:K26" si="8">G3+K3</f>
         <v>0.99470585648148147</v>
       </c>
-      <c r="L23" s="57"/>
-      <c r="N23" s="60"/>
+      <c r="L23" s="45"/>
+      <c r="N23" s="48"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J24" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="56">
+      <c r="K24" s="44">
         <f t="shared" si="8"/>
         <v>0.99470046296296288</v>
       </c>
-      <c r="L24" s="57"/>
-      <c r="N24" s="60"/>
+      <c r="L24" s="45"/>
+      <c r="N24" s="48"/>
     </row>
     <row r="25" spans="1:14" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
@@ -1809,11 +1809,11 @@
       <c r="J25" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="K25" s="56">
+      <c r="K25" s="44">
         <f t="shared" si="8"/>
         <v>0.99474508101851855</v>
       </c>
-      <c r="L25" s="57"/>
+      <c r="L25" s="45"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -1841,11 +1841,11 @@
       <c r="J26" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="56">
+      <c r="K26" s="44">
         <f t="shared" si="8"/>
         <v>0.99521690972222221</v>
       </c>
-      <c r="L26" s="57"/>
+      <c r="L26" s="45"/>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -1873,11 +1873,11 @@
       <c r="J27" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="56">
+      <c r="K27" s="44">
         <f>G7+K7</f>
         <v>0.9965018171296296</v>
       </c>
-      <c r="L27" s="57"/>
+      <c r="L27" s="45"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -1902,12 +1902,12 @@
       <c r="H28" s="11">
         <v>0.99470046296296299</v>
       </c>
-      <c r="J28" s="44" t="s">
+      <c r="J28" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="K28" s="44"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="44"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -2018,12 +2018,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J8:L8"/>
     <mergeCell ref="J28:M28"/>
     <mergeCell ref="J21:M21"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J8:L8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2081,7 +2081,7 @@
       <c r="H1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="53" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="18" t="s">
@@ -2116,7 +2116,7 @@
       <c r="H2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="49"/>
+      <c r="I2" s="54"/>
       <c r="K2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2154,7 +2154,7 @@
       <c r="H3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="49"/>
+      <c r="I3" s="54"/>
       <c r="K3" s="7" t="s">
         <v>6</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="H4" s="8">
         <v>0.99248929398148145</v>
       </c>
-      <c r="I4" s="49"/>
+      <c r="I4" s="54"/>
       <c r="K4" s="7" t="s">
         <v>7</v>
       </c>
@@ -2207,7 +2207,7 @@
       <c r="H5" s="8">
         <v>0.99250771990740738</v>
       </c>
-      <c r="I5" s="49"/>
+      <c r="I5" s="54"/>
       <c r="K5" s="7" t="s">
         <v>8</v>
       </c>
@@ -2233,7 +2233,7 @@
       <c r="H6" s="8">
         <v>0.99271962962962956</v>
       </c>
-      <c r="I6" s="49"/>
+      <c r="I6" s="54"/>
       <c r="K6" s="7" t="s">
         <v>9</v>
       </c>
@@ -2263,7 +2263,7 @@
       <c r="H7" s="8">
         <v>0.99446523148148147</v>
       </c>
-      <c r="I7" s="50"/>
+      <c r="I7" s="55"/>
       <c r="K7" s="7" t="s">
         <v>14</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="H9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="51" t="s">
+      <c r="I9" s="56" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       <c r="H10" s="9">
         <v>0.99318804398148153</v>
       </c>
-      <c r="I10" s="51"/>
+      <c r="I10" s="56"/>
       <c r="K10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2357,7 +2357,7 @@
       <c r="H11" s="9">
         <v>0.99322754629629628</v>
       </c>
-      <c r="I11" s="51"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -2380,7 +2380,7 @@
       <c r="H12" s="9">
         <v>0.9932298263888889</v>
       </c>
-      <c r="I12" s="51"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -2403,7 +2403,7 @@
       <c r="H13" s="9">
         <v>0.99325777777777768</v>
       </c>
-      <c r="I13" s="51"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -2426,7 +2426,7 @@
       <c r="H14" s="9">
         <v>0.9934952199074073</v>
       </c>
-      <c r="I14" s="51"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -2449,7 +2449,7 @@
       <c r="H15" s="9">
         <v>0.99559791666666664</v>
       </c>
-      <c r="I15" s="51"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.4">
       <c r="I16" s="6"/>
@@ -2483,7 +2483,7 @@
       <c r="H17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="52" t="s">
+      <c r="I17" s="57" t="s">
         <v>12</v>
       </c>
       <c r="K17" s="26">
@@ -2513,7 +2513,7 @@
         <f>TIME(23,51,14.216)</f>
         <v>0.99391203703703701</v>
       </c>
-      <c r="I18" s="52"/>
+      <c r="I18" s="57"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -2536,7 +2536,7 @@
       <c r="H19" s="10">
         <v>0.9939650000000001</v>
       </c>
-      <c r="I19" s="52"/>
+      <c r="I19" s="57"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
@@ -2559,7 +2559,7 @@
       <c r="H20" s="10">
         <v>0.99397041666666663</v>
       </c>
-      <c r="I20" s="52"/>
+      <c r="I20" s="57"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
@@ -2582,7 +2582,7 @@
       <c r="H21" s="10">
         <v>0.99400184027777783</v>
       </c>
-      <c r="I21" s="52"/>
+      <c r="I21" s="57"/>
       <c r="L21" s="20" t="e">
         <f>H2-H10</f>
         <v>#VALUE!</v>
@@ -2609,7 +2609,7 @@
       <c r="H22" s="10">
         <v>0.99429040509259259</v>
       </c>
-      <c r="I22" s="52"/>
+      <c r="I22" s="57"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -2632,7 +2632,7 @@
       <c r="H23" s="10">
         <v>0.99650180555555556</v>
       </c>
-      <c r="I23" s="52"/>
+      <c r="I23" s="57"/>
     </row>
     <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.4">
       <c r="I24" s="6"/>
@@ -2658,7 +2658,7 @@
       <c r="H25" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="53" t="s">
+      <c r="I25" s="58" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       <c r="H26" s="11">
         <v>0.99464123842592589</v>
       </c>
-      <c r="I26" s="54"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -2706,7 +2706,7 @@
       <c r="H27" s="11">
         <v>0.99470585648148147</v>
       </c>
-      <c r="I27" s="54"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -2729,7 +2729,7 @@
       <c r="H28" s="11">
         <v>0.99470046296296299</v>
       </c>
-      <c r="I28" s="54"/>
+      <c r="I28" s="59"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -2752,7 +2752,7 @@
       <c r="H29" s="11">
         <v>0.99474508101851855</v>
       </c>
-      <c r="I29" s="54"/>
+      <c r="I29" s="59"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -2775,7 +2775,7 @@
       <c r="H30" s="11">
         <v>0.99521690972222221</v>
       </c>
-      <c r="I30" s="54"/>
+      <c r="I30" s="59"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -2790,7 +2790,7 @@
       <c r="F31" s="23"/>
       <c r="G31" s="5"/>
       <c r="H31" s="11"/>
-      <c r="I31" s="55"/>
+      <c r="I31" s="60"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>

</xml_diff>